<commit_message>
feature: add final project:
</commit_message>
<xml_diff>
--- a/res/cardiological_minsize.xlsx
+++ b/res/cardiological_minsize.xlsx
@@ -371,17 +371,39 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.801303488973446</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.23404690932392</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.846169544288195</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.719339596926695</v>
-      </c>
-      <c r="C2" t="n">
-        <v>6.47688748427627</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.773902385691451</v>
-      </c>
+      <c r="B3" t="n">
+        <v>0.657822406125166</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.99923359854542</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.731450191729779</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>